<commit_message>
+ Days per week
</commit_message>
<xml_diff>
--- a/lab_files/telework_cases.xlsx
+++ b/lab_files/telework_cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc.mouries/projects/Telework-Case-Management-Lab/lab_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AC19DD-B779-9A4B-91DD-2B71750DFE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85C426B-7FE1-7F4A-85B2-298EF9D4396D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36600" yWindow="5940" windowWidth="34560" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36580" yWindow="5880" windowWidth="34560" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="65">
   <si>
     <t>Priority</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>Dependent Care</t>
+  </si>
+  <si>
+    <t>Days per week</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -276,13 +282,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D147A1B0-A85F-FA48-A1C5-41EB9223ECB6}" name="Table3" displayName="Table3" ref="A1:G40" totalsRowShown="0">
-  <autoFilter ref="A1:G40" xr:uid="{D147A1B0-A85F-FA48-A1C5-41EB9223ECB6}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D147A1B0-A85F-FA48-A1C5-41EB9223ECB6}" name="Table3" displayName="Table3" ref="A1:H40" totalsRowShown="0">
+  <autoFilter ref="A1:H40" xr:uid="{D147A1B0-A85F-FA48-A1C5-41EB9223ECB6}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{0C012D46-43FC-2E47-9135-64C87BC989F7}" name="Priority"/>
     <tableColumn id="2" xr3:uid="{8268E2B7-8F23-CD46-8AC7-BE2BB9EC75FB}" name="Opened by"/>
     <tableColumn id="3" xr3:uid="{23A92060-4CF4-3D4F-AF49-D87B20399EAE}" name="Arrangement"/>
     <tableColumn id="4" xr3:uid="{90B0A2D0-33F0-2C4B-9327-6D94DBF7FBBA}" name="Reason"/>
+    <tableColumn id="8" xr3:uid="{13634DD4-BDB0-6145-802D-603B57CA3061}" name="Days per week"/>
     <tableColumn id="5" xr3:uid="{B8435C68-C517-2D40-8F8E-473D26479298}" name="Short description"/>
     <tableColumn id="6" xr3:uid="{EC84D9EF-21DB-4646-84C1-4DAF1D4426BD}" name="State"/>
     <tableColumn id="7" xr3:uid="{29E0F2D8-D675-914F-BE2C-C1EBB02971A1}" name="Assigned to"/>
@@ -588,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964130B9-ACDF-8E40-967F-916E8D66C226}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -600,12 +607,13 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -619,16 +627,19 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -636,19 +647,22 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -656,19 +670,22 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -682,16 +699,19 @@
         <v>43</v>
       </c>
       <c r="E4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -705,16 +725,19 @@
         <v>62</v>
       </c>
       <c r="E5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -728,13 +751,16 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -748,13 +774,16 @@
         <v>43</v>
       </c>
       <c r="E7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -768,13 +797,16 @@
         <v>43</v>
       </c>
       <c r="E8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -787,14 +819,17 @@
       <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -808,13 +843,16 @@
         <v>43</v>
       </c>
       <c r="E10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -828,13 +866,16 @@
         <v>43</v>
       </c>
       <c r="E11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -848,13 +889,16 @@
         <v>43</v>
       </c>
       <c r="E12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -868,16 +912,19 @@
         <v>43</v>
       </c>
       <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
         <v>37</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>11</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -891,16 +938,19 @@
         <v>43</v>
       </c>
       <c r="E14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
         <v>38</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>11</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -913,17 +963,20 @@
       <c r="D15" t="s">
         <v>53</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15" t="s">
         <v>39</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>18</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -936,14 +989,17 @@
       <c r="D16" t="s">
         <v>62</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
         <v>41</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -956,14 +1012,17 @@
       <c r="D17" t="s">
         <v>62</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
         <v>42</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -976,17 +1035,20 @@
       <c r="D18" t="s">
         <v>43</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
         <v>44</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>18</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -999,17 +1061,20 @@
       <c r="D19" t="s">
         <v>43</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>45</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>11</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1022,17 +1087,20 @@
       <c r="D20" t="s">
         <v>43</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
         <v>46</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>11</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1046,13 +1114,16 @@
         <v>43</v>
       </c>
       <c r="E21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" t="s">
         <v>23</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1066,16 +1137,19 @@
         <v>43</v>
       </c>
       <c r="E22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" t="s">
         <v>49</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>18</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1089,16 +1163,19 @@
         <v>43</v>
       </c>
       <c r="E23" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" t="s">
         <v>50</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>18</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -1111,17 +1188,20 @@
       <c r="D24" t="s">
         <v>43</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>51</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>18</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1134,17 +1214,20 @@
       <c r="D25" t="s">
         <v>43</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
         <v>52</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>11</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1158,16 +1241,19 @@
         <v>53</v>
       </c>
       <c r="E26" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" t="s">
         <v>30</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>48</v>
       </c>
@@ -1181,16 +1267,19 @@
         <v>43</v>
       </c>
       <c r="E27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" t="s">
         <v>29</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>20</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1204,16 +1293,19 @@
         <v>53</v>
       </c>
       <c r="E28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" t="s">
         <v>54</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>20</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>55</v>
       </c>
@@ -1227,13 +1319,16 @@
         <v>43</v>
       </c>
       <c r="E29" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" t="s">
         <v>57</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1246,17 +1341,20 @@
       <c r="D30" t="s">
         <v>43</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
         <v>58</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>11</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1269,17 +1367,20 @@
       <c r="D31" t="s">
         <v>43</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
         <v>10</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>20</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1293,16 +1394,19 @@
         <v>53</v>
       </c>
       <c r="E32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" t="s">
         <v>32</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>18</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1316,16 +1420,19 @@
         <v>53</v>
       </c>
       <c r="E33" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" t="s">
         <v>41</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>18</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -1339,16 +1446,19 @@
         <v>53</v>
       </c>
       <c r="E34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" t="s">
         <v>42</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>11</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -1362,13 +1472,16 @@
         <v>53</v>
       </c>
       <c r="E35" t="s">
+        <v>64</v>
+      </c>
+      <c r="F35" t="s">
         <v>25</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -1382,13 +1495,16 @@
         <v>53</v>
       </c>
       <c r="E36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" t="s">
         <v>27</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -1402,13 +1518,16 @@
         <v>53</v>
       </c>
       <c r="E37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" t="s">
         <v>57</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -1422,13 +1541,16 @@
         <v>53</v>
       </c>
       <c r="E38" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" t="s">
         <v>34</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -1442,16 +1564,19 @@
         <v>53</v>
       </c>
       <c r="E39" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" t="s">
         <v>60</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>20</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -1465,12 +1590,15 @@
         <v>53</v>
       </c>
       <c r="E40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" t="s">
         <v>61</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>20</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>